<commit_message>
Fund Center and IT calculator update
</commit_message>
<xml_diff>
--- a/TestData/ITCalculator_TestData.xlsx
+++ b/TestData/ITCalculator_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="192">
   <si>
     <t>Age</t>
   </si>
@@ -593,13 +593,18 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Actual IT</t>
+  </si>
+  <si>
+    <t>Actual Net Sal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -946,23 +951,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD706"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="36.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -978,8 +984,17 @@
       <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -996,7 +1011,7 @@
         <v>21119.19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1013,7 +1028,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1030,7 +1045,7 @@
         <v>6925</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1047,7 +1062,7 @@
         <v>32693.78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1064,7 +1079,7 @@
         <v>28109.19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1096,7 @@
         <v>43874.28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1098,7 +1113,7 @@
         <v>43280.04</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1106,7 +1121,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="1">
-        <v>1500001</v>
+        <v>150000.01</v>
       </c>
       <c r="D9" s="1">
         <v>42734.42</v>
@@ -1115,7 +1130,7 @@
         <v>82265.66</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1132,7 +1147,7 @@
         <v>28792.44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1149,7 +1164,7 @@
         <v>10720.83</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1166,7 +1181,7 @@
         <v>10720.83</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1183,7 +1198,7 @@
         <v>44023.78</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1200,7 +1215,7 @@
         <v>41507.53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1232,7 @@
         <v>36577.03</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1242,7 +1257,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="1">
-        <v>1500003</v>
+        <v>15000.03</v>
       </c>
       <c r="D17" s="1">
         <v>42051.24</v>
@@ -1404,29 +1419,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="20" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>